<commit_message>
updated and not finished gantt chart
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22729"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Secundu\Soft Eng\proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\DaciaSandero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_9B76E24B249114BC1F35B6FAE11353D450B7C846" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{42BCF56B-9C27-4D31-B5A9-3BC70FDAD178}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Before covid" sheetId="1" r:id="rId1"/>
+    <sheet name="After Covid" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>Date commencing</t>
   </si>
@@ -234,13 +234,64 @@
   </si>
   <si>
     <t>enhance existing solutions</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Ideation</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Iterative</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Mathematical</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>final touches</t>
+  </si>
+  <si>
+    <t>find new dataset</t>
+  </si>
+  <si>
+    <t>setup detection in one file</t>
+  </si>
+  <si>
+    <t>setup environment</t>
+  </si>
+  <si>
+    <t>setup training</t>
+  </si>
+  <si>
+    <t>evaluate detection</t>
+  </si>
+  <si>
+    <t>evaluate training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,14 +646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
@@ -618,7 +669,7 @@
     <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +707,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -694,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -710,7 +761,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="G4" s="1"/>
@@ -720,14 +771,14 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -736,26 +787,26 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -766,7 +817,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -779,7 +830,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -792,12 +843,12 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -823,7 +874,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -849,7 +900,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -873,7 +924,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -895,7 +946,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -915,7 +966,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -933,7 +984,7 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -959,7 +1010,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -979,7 +1030,7 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1001,7 +1052,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
         <v>10</v>
@@ -1020,7 +1071,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>30</v>
       </c>
@@ -1028,37 +1079,37 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1078,7 +1129,7 @@
         <v>43926</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +1143,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>43</v>
       </c>
@@ -1106,7 +1157,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>47</v>
       </c>
@@ -1120,7 +1171,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>51</v>
       </c>
@@ -1131,7 +1182,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>54</v>
       </c>
@@ -1142,7 +1193,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>57</v>
       </c>
@@ -1150,7 +1201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>59</v>
       </c>
@@ -1161,7 +1212,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>62</v>
       </c>
@@ -1169,7 +1220,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>64</v>
       </c>
@@ -1177,7 +1228,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>66</v>
       </c>
@@ -1189,4 +1240,147 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="7">
+        <v>43934</v>
+      </c>
+      <c r="C2" s="7">
+        <v>43941</v>
+      </c>
+      <c r="D2" s="7">
+        <v>43948</v>
+      </c>
+      <c r="E2" s="7">
+        <v>43955</v>
+      </c>
+      <c r="F2" s="7">
+        <v>43962</v>
+      </c>
+      <c r="G2" s="7">
+        <v>43969</v>
+      </c>
+      <c r="H2" s="7">
+        <v>43976</v>
+      </c>
+      <c r="I2" s="7">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to Team Management and detection setup
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Date commencing</t>
   </si>
@@ -146,96 +146,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Date of meeting</t>
-  </si>
-  <si>
-    <t>19/02</t>
-  </si>
-  <si>
-    <t>ideas</t>
-  </si>
-  <si>
-    <t>gantt chart</t>
-  </si>
-  <si>
-    <t>settled on theme</t>
-  </si>
-  <si>
-    <t>1pm- 3pm</t>
-  </si>
-  <si>
-    <t>missions</t>
-  </si>
-  <si>
-    <t>checkpoints</t>
-  </si>
-  <si>
-    <t>video research</t>
-  </si>
-  <si>
-    <t>got github working</t>
-  </si>
-  <si>
-    <t>proposal review</t>
-  </si>
-  <si>
-    <t>dataset search</t>
-  </si>
-  <si>
-    <t>algorithm search</t>
-  </si>
-  <si>
-    <t>Mircea got Anaconda</t>
-  </si>
-  <si>
-    <t>algorithm doc</t>
-  </si>
-  <si>
-    <t>new task: advanced gantt</t>
-  </si>
-  <si>
-    <t>installing keras</t>
-  </si>
-  <si>
-    <t>github setup</t>
-  </si>
-  <si>
-    <t>api reseach</t>
-  </si>
-  <si>
-    <t>opencv</t>
-  </si>
-  <si>
-    <t>agreed to delay until</t>
-  </si>
-  <si>
-    <t>tkinter</t>
-  </si>
-  <si>
-    <t>add "stuff we tried"</t>
-  </si>
-  <si>
-    <t>intelligent systems is finished</t>
-  </si>
-  <si>
-    <t>tensorflow</t>
-  </si>
-  <si>
-    <t>document the process</t>
-  </si>
-  <si>
-    <t>coronavirus</t>
-  </si>
-  <si>
-    <t>YOLO + SSD</t>
-  </si>
-  <si>
-    <t>boosted to a meeting every other day</t>
-  </si>
-  <si>
-    <t>enhance existing solutions</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -285,6 +195,12 @@
   </si>
   <si>
     <t>evaluate training</t>
+  </si>
+  <si>
+    <t>bulk of writing</t>
+  </si>
+  <si>
+    <t>have diagram prepared</t>
   </si>
 </sst>
 </file>
@@ -647,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,129 +1025,11 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="7">
-        <v>43886</v>
-      </c>
-      <c r="D34" s="7">
-        <v>43893</v>
-      </c>
-      <c r="F34" s="7">
-        <v>43900</v>
-      </c>
-      <c r="H34" s="7">
-        <v>43926</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" t="s">
-        <v>41</v>
-      </c>
-      <c r="H35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38" t="s">
-        <v>52</v>
-      </c>
-      <c r="H38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-      <c r="F39" t="s">
-        <v>55</v>
-      </c>
-      <c r="H39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F40" t="s">
-        <v>57</v>
-      </c>
-      <c r="H40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" t="s">
-        <v>60</v>
-      </c>
-      <c r="H41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>62</v>
-      </c>
-      <c r="H42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>66</v>
-      </c>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="H34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1247,7 +1045,7 @@
   <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,12 +1055,15 @@
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7">
         <v>43934</v>
@@ -1291,92 +1092,101 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>